<commit_message>
segunda version - se modifica dias atraso credito 148
</commit_message>
<xml_diff>
--- a/Clasificacion_deudor.xlsx
+++ b/Clasificacion_deudor.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/016b0726b02d19b5/Documentos/Capacitación/202302 CERTUS Data Analitycs/UD3 DataOps/UD3_S03_20230525/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fredg\workspace\tarea_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="8_{B02CB419-8EAB-4DF0-8217-55D36E033AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{696704FC-24D7-42A2-A804-DAFEDE48341F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A969C512-EC2F-408F-8EEF-1D6668BDCBC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6C1FE71-EB55-4080-B2BE-8A85D8AAF5F7}"/>
   </bookViews>
@@ -241,10 +241,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -550,7 +546,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -606,15 +602,15 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F2" s="3" t="str">
         <f>IF($E2&lt;=8,"A",IF($E2&lt;=30,"B",IF($E2&lt;=60,"C",IF($E2&lt;=120,"D","E"))))</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="G2" s="3" t="str">
         <f t="array" ref="G2">CHAR(MAX(IF($B$2:$B$10=B2,CODE($F$2:$F$10))))</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="H2" s="2">
         <v>1022.3</v>

</xml_diff>